<commit_message>
Add result view and update UI logic
</commit_message>
<xml_diff>
--- a/assets/data/puzzle_list.xlsx
+++ b/assets/data/puzzle_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Projects/puzzility/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC09087-AD6F-EC4A-A00F-1819AB9C3CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CCCC39-46DA-D040-8250-82B136AD0537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>No</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>A,B,C,D</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>That is brilliant! You only need to do it once. How amazing that is!</t>
+  </si>
+  <si>
+    <t>That is correct!, wish we could cut our own hair like a pro</t>
   </si>
 </sst>
 </file>
@@ -380,10 +389,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -391,7 +400,7 @@
     <col min="3" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +428,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -446,8 +458,11 @@
       <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -475,8 +490,11 @@
       <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J3" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
@@ -487,7 +505,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7"/>
@@ -498,7 +516,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -509,7 +527,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -520,7 +538,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -531,7 +549,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -542,7 +560,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -553,7 +571,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -564,7 +582,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -575,7 +593,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -586,7 +604,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -597,7 +615,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -608,7 +626,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>